<commit_message>
Fixing input data for some tests.
</commit_message>
<xml_diff>
--- a/tests/models/features/multiple_problems/input_data/input_data.xlsx
+++ b/tests/models/features/multiple_problems/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\features\multiple_problems\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFC6E67-10D2-4287-B5B5-D8C370483EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4957C91C-AFF1-406B-90D9-3C51FB89DFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13380" yWindow="4920" windowWidth="10700" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_constraints" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>products</t>
-  </si>
-  <si>
     <t>values</t>
   </si>
   <si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>product 2</t>
+  </si>
+  <si>
+    <t>p_Names</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,10 +410,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -421,7 +421,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>15</v>
@@ -432,7 +432,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>10</v>

</xml_diff>

<commit_message>
Updating settings for 'multiple_problems' and '1_coupled_model' test cases.
</commit_message>
<xml_diff>
--- a/tests/models/features/multiple_problems/input_data/input_data.xlsx
+++ b/tests/models/features/multiple_problems/input_data/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\features\multiple_problems\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4957C91C-AFF1-406B-90D9-3C51FB89DFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25D4130-C5CA-49BA-AA50-B4A2B3EBE0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_constraints" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,9 @@
     <t>id</t>
   </si>
   <si>
+    <t>products_Name</t>
+  </si>
+  <si>
     <t>values</t>
   </si>
   <si>
@@ -32,9 +35,6 @@
   </si>
   <si>
     <t>product 2</t>
-  </si>
-  <si>
-    <t>p_Names</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,10 +410,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -421,10 +421,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -432,10 +432,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>